<commit_message>
feat: adcionado sistema executavel
</commit_message>
<xml_diff>
--- a/tarefa.xlsx
+++ b/tarefa.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,26 +454,69 @@
           <t>status</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>historico</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>a</t>
+          <t xml:space="preserve">a </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>a</t>
+          <t xml:space="preserve">a </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0:00:19.583634</t>
+          <t>0:00:09.036521</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Pausada</t>
+          <t>Finalizada</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Iniciada em: 23:10:01
+Pausada em: 23:10:06
+Iniciada em: 23:14:57
+Pausada em: 23:15:02
+Finalizada em: 23:15:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0:00:04.326423</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Finalizada</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Iniciada em: 23:16:06
+Pausada em: 23:16:10
+Finalizada em: 23:16:16</t>
         </is>
       </c>
     </row>

</xml_diff>